<commit_message>
Overlapping times are correctly calculated [Fixes #1]
</commit_message>
<xml_diff>
--- a/testfile-zoom_participants_93522834467.xlsx
+++ b/testfile-zoom_participants_93522834467.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ysbach/Dropbox/github/snuetl-attchk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CEA2C4-112E-4A4F-BFCD-D07859146EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A045F21-6532-FA43-8E0A-7D7B95CB0BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2160" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participants" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>ID number</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>2019-11111</t>
-  </si>
-  <si>
-    <t>2018-11111</t>
   </si>
   <si>
     <t>오오오</t>
@@ -564,12 +561,14 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="52.5" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -710,13 +709,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>23</v>
@@ -730,13 +729,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>28</v>
@@ -750,10 +749,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>50</v>
@@ -809,8 +808,8 @@
     <hyperlink ref="C6" r:id="rId4" xr:uid="{902B2215-0173-EA46-ACFC-57F09EFE817D}"/>
     <hyperlink ref="C7" r:id="rId5" xr:uid="{B1C6FED2-C191-5A49-8AA3-79D117A6844B}"/>
     <hyperlink ref="C9" r:id="rId6" xr:uid="{4951743C-0C34-FB4D-991A-4DDA9DA5351D}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{22931096-69FE-D54B-8B25-AF26D14FD936}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{9E6FBC7C-2F0B-BD4B-82A2-7270A0CE51C0}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{9E6FBC7C-2F0B-BD4B-82A2-7270A0CE51C0}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{F4F6E5F4-89C9-5741-BDCA-5DA5ED679C94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>